<commit_message>
make dem/gop footnote fields, make them conditional on results display
</commit_message>
<xml_diff>
--- a/data/copy.xlsx
+++ b/data/copy.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="123">
   <si>
     <t>key</t>
   </si>
@@ -33,22 +33,13 @@
     <t>Elections 2016</t>
   </si>
   <si>
-    <t>iowa_dem_disclaimer</t>
+    <t>results_gop_footnote</t>
   </si>
   <si>
-    <t>Democratic vote totals are "state delegate equivalents" -- an estimated number of delegates that will be sent to county and state conventions to formally select the delegates who will represent Iowa and the winning candidates at the national convention. Democrats do not immediately report the raw vote and never report what share of the raw vote each candidate&amp;nbsp;won.</t>
+    <t>Test GOP</t>
   </si>
   <si>
-    <t>nev_dem_disclaimer</t>
-  </si>
-  <si>
-    <t>Democratic vote totals are numbers of delegates who will attend county party conventions. The party does not report the raw&amp;nbsp;vote.</t>
-  </si>
-  <si>
-    <t>nev_gop_disclaimer</t>
-  </si>
-  <si>
-    <t>Polls close in South Carolina at 7 p.m. EST.</t>
+    <t>results_dem_footnote</t>
   </si>
   <si>
     <t>delegates_dem_footnote</t>
@@ -608,31 +599,32 @@
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="B4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -643,42 +635,31 @@
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="A11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" s="2"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -694,126 +675,126 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -830,117 +811,117 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -964,13 +945,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
@@ -998,86 +979,86 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1125,10 +1106,10 @@
     </row>
     <row r="2" ht="30.0" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -1151,10 +1132,10 @@
     </row>
     <row r="3" ht="30.0" customHeight="1">
       <c r="A3" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -1177,10 +1158,10 @@
     </row>
     <row r="4" ht="30.0" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
@@ -1203,10 +1184,10 @@
     </row>
     <row r="5" ht="30.0" customHeight="1">
       <c r="A5" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
@@ -1229,10 +1210,10 @@
     </row>
     <row r="6" ht="30.0" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
@@ -1255,7 +1236,7 @@
     </row>
     <row r="7" ht="30.0" customHeight="1">
       <c r="A7" s="9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>3</v>
@@ -1281,10 +1262,10 @@
     </row>
     <row r="8" ht="30.0" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
@@ -1307,10 +1288,10 @@
     </row>
     <row r="9" ht="30.0" customHeight="1">
       <c r="A9" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -1333,10 +1314,10 @@
     </row>
     <row r="10" ht="30.0" customHeight="1">
       <c r="A10" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -1359,10 +1340,10 @@
     </row>
     <row r="11" ht="30.0" customHeight="1">
       <c r="A11" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -1385,7 +1366,7 @@
     </row>
     <row r="12" ht="30.0" customHeight="1">
       <c r="A12" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -1409,7 +1390,7 @@
     </row>
     <row r="13" ht="30.0" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -1433,7 +1414,7 @@
     </row>
     <row r="14" ht="30.0" customHeight="1">
       <c r="A14" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -1457,7 +1438,7 @@
     </row>
     <row r="15" ht="30.0" customHeight="1">
       <c r="A15" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -1481,7 +1462,7 @@
     </row>
     <row r="16" ht="30.0" customHeight="1">
       <c r="A16" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -1505,7 +1486,7 @@
     </row>
     <row r="17" ht="30.0" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -1529,10 +1510,10 @@
     </row>
     <row r="18" ht="30.0" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -1555,10 +1536,10 @@
     </row>
     <row r="19" ht="30.0" customHeight="1">
       <c r="A19" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
@@ -1581,10 +1562,10 @@
     </row>
     <row r="20" ht="30.0" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -1607,10 +1588,10 @@
     </row>
     <row r="21" ht="30.0" customHeight="1">
       <c r="A21" s="9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
@@ -3510,42 +3491,42 @@
     </row>
     <row r="2" ht="33.0" customHeight="1">
       <c r="A2" s="17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" ht="33.0" customHeight="1">
       <c r="A3" s="17" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" ht="33.0" customHeight="1">
       <c r="A4" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" ht="33.0" customHeight="1">
       <c r="A5" s="17" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" ht="33.0" customHeight="1">
       <c r="A6" s="17" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" ht="33.0" customHeight="1">
@@ -7546,58 +7527,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -7626,50 +7607,50 @@
     </row>
     <row r="2">
       <c r="A2" s="20" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="20" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="20" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="20" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="20" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8">
@@ -11666,34 +11647,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="19" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="20" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="20" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="20" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
adjust logic for titlecard button text
</commit_message>
<xml_diff>
--- a/data/copy.xlsx
+++ b/data/copy.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="128">
   <si>
     <t>key</t>
   </si>
@@ -37,22 +37,22 @@
     <t>prod_state</t>
   </si>
   <si>
-    <t>before</t>
+    <t>after</t>
   </si>
   <si>
     <t>stage_state</t>
   </si>
   <si>
-    <t>dev_state</t>
+    <t>during</t>
   </si>
   <si>
-    <t>during</t>
+    <t>dev_state</t>
   </si>
   <si>
     <t>live_audio</t>
   </si>
   <si>
-    <t>live</t>
+    <t>inactive</t>
   </si>
   <si>
     <t>results_gop_footnote</t>
@@ -76,7 +76,7 @@
     <t>delegates_gop_footnote</t>
   </si>
   <si>
-    <t>Jeb Bush, Carly Fiorina and Rand Paul suspended their campaigns.</t>
+    <t>Jeb Bush, Carly Fiorina, Mike Huckabee and Rand Paul suspended their campaigns.</t>
   </si>
   <si>
     <t>donate_hed</t>
@@ -391,16 +391,22 @@
     <t>states</t>
   </si>
   <si>
-    <t>Tuesday, March 1</t>
-  </si>
-  <si>
-    <t>&lt;strong&gt;Super Tuesday&lt;/strong&gt;: Alabama, Alaska (R), Arkansas, Colorado, Georgia, Massachusetts, Minnesota, Oklahoma, Tennessee, Texas, Vermont, Virginia, Wyoming (R), American Samoa (D), Democrats Abroad</t>
-  </si>
-  <si>
     <t>Saturday, March 5</t>
   </si>
   <si>
     <t>Kansas, Kentucky (R), Louisiana, Maine (R), Nebraska (D)</t>
+  </si>
+  <si>
+    <t>Sunday, March 6</t>
+  </si>
+  <si>
+    <t>Maine (D), Puerto Rico (R)</t>
+  </si>
+  <si>
+    <t>Tuesday, March 8</t>
+  </si>
+  <si>
+    <t>Hawaii (R), Idaho (R), Michigan, Mississippi</t>
   </si>
 </sst>
 </file>
@@ -631,15 +637,15 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -737,11 +743,19 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="2" t="s">
         <v>125</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="5">
@@ -4723,10 +4737,6 @@
     <row r="999">
       <c r="A999" s="22"/>
       <c r="B999" s="22"/>
-    </row>
-    <row r="1000">
-      <c r="A1000" s="22"/>
-      <c r="B1000" s="22"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -5042,67 +5052,78 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>49</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update podcast for after mode
</commit_message>
<xml_diff>
--- a/data/copy.xlsx
+++ b/data/copy.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="128">
   <si>
     <t>key</t>
   </si>
@@ -645,7 +645,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -5043,87 +5043,96 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>37</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C4" s="5"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>49</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
working tests, but it is sloooow
</commit_message>
<xml_diff>
--- a/data/copy.xlsx
+++ b/data/copy.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="186">
   <si>
     <t>key</t>
   </si>
@@ -256,9 +256,6 @@
     <t>Republican Results</t>
   </si>
   <si>
-    <t>Democratic Results</t>
-  </si>
-  <si>
     <t>Get Caught Up</t>
   </si>
   <si>
@@ -392,6 +389,9 @@
   </si>
   <si>
     <t>what_happened</t>
+  </si>
+  <si>
+    <t>Democratic Results</t>
   </si>
   <si>
     <t>error_headline</t>
@@ -9135,7 +9135,7 @@
         <v>172</v>
       </c>
       <c r="B6" s="42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7">
@@ -9171,18 +9171,18 @@
         <v>53</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="42" t="s">
         <v>177</v>
@@ -9191,12 +9191,12 @@
         <v>178</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="41" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3" s="42" t="s">
         <v>179</v>
@@ -9208,7 +9208,7 @@
     </row>
     <row r="4">
       <c r="A4" s="41" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4" s="42" t="s">
         <v>181</v>
@@ -9220,19 +9220,19 @@
     </row>
     <row r="5">
       <c r="A5" s="41" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" s="42" t="s">
         <v>183</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D5" s="43"/>
     </row>
     <row r="6">
       <c r="A6" s="41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" s="42" t="s">
         <v>184</v>
@@ -11813,73 +11813,62 @@
         <v>77</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>62</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="C6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -11900,31 +11889,31 @@
         <v>53</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="F1" s="16"/>
       <c r="G1" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="I1" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="J1" s="17" t="s">
         <v>85</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="19" t="str">
         <f t="shared" ref="B2:B5" si="1">H2</f>
@@ -11935,11 +11924,11 @@
         <v>71.2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F2" s="21"/>
       <c r="G2" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H2" s="23">
         <v>24787.0</v>
@@ -11953,7 +11942,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3" s="19" t="str">
         <f t="shared" si="1"/>
@@ -11965,7 +11954,7 @@
       </c>
       <c r="F3" s="21"/>
       <c r="G3" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H3" s="23">
         <v>4479.0</v>
@@ -11979,7 +11968,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4" s="19" t="str">
         <f t="shared" si="1"/>
@@ -11991,7 +11980,7 @@
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H4" s="23">
         <v>2903.0</v>
@@ -12005,7 +11994,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" s="19" t="str">
         <f t="shared" si="1"/>
@@ -12017,7 +12006,7 @@
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H5" s="23">
         <v>450.0</v>
@@ -12031,7 +12020,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" s="25" t="str">
         <f>sum(H6:H14)</f>
@@ -12043,7 +12032,7 @@
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H6" s="23">
         <v>273.0</v>
@@ -12066,7 +12055,7 @@
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H7" s="23">
         <v>229.0</v>
@@ -12082,7 +12071,7 @@
       <c r="B8" s="27"/>
       <c r="F8" s="21"/>
       <c r="G8" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H8" s="23">
         <v>125.0</v>
@@ -12098,7 +12087,7 @@
       <c r="B9" s="27"/>
       <c r="F9" s="21"/>
       <c r="G9" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H9" s="23">
         <v>58.0</v>
@@ -12114,7 +12103,7 @@
       <c r="B10" s="27"/>
       <c r="F10" s="21"/>
       <c r="G10" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H10" s="23">
         <v>39.0</v>
@@ -12128,21 +12117,21 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="E11" s="30"/>
       <c r="F11" s="21"/>
       <c r="G11" s="22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H11" s="23">
         <v>28.0</v>
@@ -12156,18 +12145,18 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B12" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" s="29" t="s">
         <v>105</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>106</v>
       </c>
       <c r="E12" s="30"/>
       <c r="F12" s="21"/>
       <c r="G12" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H12" s="23">
         <v>25.0</v>
@@ -12181,18 +12170,18 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B13" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="29" t="s">
         <v>108</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>109</v>
       </c>
       <c r="E13" s="30"/>
       <c r="F13" s="21"/>
       <c r="G13" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H13" s="23">
         <v>19.0</v>
@@ -12206,18 +12195,18 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B14" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="29" t="s">
         <v>111</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>112</v>
       </c>
       <c r="E14" s="30"/>
       <c r="F14" s="21"/>
       <c r="G14" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H14" s="23">
         <v>1413.0</v>
@@ -12226,28 +12215,28 @@
         <v>4.0E-4</v>
       </c>
       <c r="J14" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B15" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>116</v>
       </c>
       <c r="E15" s="30"/>
       <c r="H15" s="32"/>
     </row>
     <row r="16">
       <c r="B16" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" s="30" t="s">
         <v>117</v>
-      </c>
-      <c r="C16" s="30" t="s">
-        <v>118</v>
       </c>
       <c r="H16" s="32"/>
     </row>
@@ -16263,19 +16252,19 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -16292,7 +16281,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
desktop design of combined live audio/what's happening card
</commit_message>
<xml_diff>
--- a/data/copy.xlsx
+++ b/data/copy.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="186">
   <si>
     <t>key</t>
   </si>
@@ -256,9 +256,6 @@
     <t>Republican Results</t>
   </si>
   <si>
-    <t>Democratic Results</t>
-  </si>
-  <si>
     <t>Get Caught Up</t>
   </si>
   <si>
@@ -392,6 +389,9 @@
   </si>
   <si>
     <t>what_happened</t>
+  </si>
+  <si>
+    <t>Democratic Results</t>
   </si>
   <si>
     <t>error_headline</t>
@@ -9135,7 +9135,7 @@
         <v>172</v>
       </c>
       <c r="B6" s="42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7">
@@ -9171,18 +9171,18 @@
         <v>53</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="42" t="s">
         <v>177</v>
@@ -9191,12 +9191,12 @@
         <v>178</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="41" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3" s="42" t="s">
         <v>179</v>
@@ -9208,7 +9208,7 @@
     </row>
     <row r="4">
       <c r="A4" s="41" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4" s="42" t="s">
         <v>181</v>
@@ -9220,19 +9220,19 @@
     </row>
     <row r="5">
       <c r="A5" s="41" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" s="42" t="s">
         <v>183</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D5" s="43"/>
     </row>
     <row r="6">
       <c r="A6" s="41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" s="42" t="s">
         <v>184</v>
@@ -11813,73 +11813,62 @@
         <v>77</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>62</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="C6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="2" t="s">
         <v>74</v>
       </c>
     </row>
@@ -11900,31 +11889,31 @@
         <v>53</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="F1" s="16"/>
       <c r="G1" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="I1" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="J1" s="17" t="s">
         <v>85</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="19" t="str">
         <f t="shared" ref="B2:B5" si="1">H2</f>
@@ -11935,11 +11924,11 @@
         <v>71.2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F2" s="21"/>
       <c r="G2" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H2" s="23">
         <v>24787.0</v>
@@ -11953,7 +11942,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3" s="19" t="str">
         <f t="shared" si="1"/>
@@ -11965,7 +11954,7 @@
       </c>
       <c r="F3" s="21"/>
       <c r="G3" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H3" s="23">
         <v>4479.0</v>
@@ -11979,7 +11968,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4" s="19" t="str">
         <f t="shared" si="1"/>
@@ -11991,7 +11980,7 @@
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H4" s="23">
         <v>2903.0</v>
@@ -12005,7 +11994,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" s="19" t="str">
         <f t="shared" si="1"/>
@@ -12017,7 +12006,7 @@
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H5" s="23">
         <v>450.0</v>
@@ -12031,7 +12020,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B6" s="25" t="str">
         <f>sum(H6:H14)</f>
@@ -12043,7 +12032,7 @@
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H6" s="23">
         <v>273.0</v>
@@ -12066,7 +12055,7 @@
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H7" s="23">
         <v>229.0</v>
@@ -12082,7 +12071,7 @@
       <c r="B8" s="27"/>
       <c r="F8" s="21"/>
       <c r="G8" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H8" s="23">
         <v>125.0</v>
@@ -12098,7 +12087,7 @@
       <c r="B9" s="27"/>
       <c r="F9" s="21"/>
       <c r="G9" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H9" s="23">
         <v>58.0</v>
@@ -12114,7 +12103,7 @@
       <c r="B10" s="27"/>
       <c r="F10" s="21"/>
       <c r="G10" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H10" s="23">
         <v>39.0</v>
@@ -12128,21 +12117,21 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>88</v>
       </c>
       <c r="E11" s="30"/>
       <c r="F11" s="21"/>
       <c r="G11" s="22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H11" s="23">
         <v>28.0</v>
@@ -12156,18 +12145,18 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B12" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" s="29" t="s">
         <v>105</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>106</v>
       </c>
       <c r="E12" s="30"/>
       <c r="F12" s="21"/>
       <c r="G12" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H12" s="23">
         <v>25.0</v>
@@ -12181,18 +12170,18 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B13" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="29" t="s">
         <v>108</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>109</v>
       </c>
       <c r="E13" s="30"/>
       <c r="F13" s="21"/>
       <c r="G13" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H13" s="23">
         <v>19.0</v>
@@ -12206,18 +12195,18 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B14" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="29" t="s">
         <v>111</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>112</v>
       </c>
       <c r="E14" s="30"/>
       <c r="F14" s="21"/>
       <c r="G14" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H14" s="23">
         <v>1413.0</v>
@@ -12226,28 +12215,28 @@
         <v>4.0E-4</v>
       </c>
       <c r="J14" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B15" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>116</v>
       </c>
       <c r="E15" s="30"/>
       <c r="H15" s="32"/>
     </row>
     <row r="16">
       <c r="B16" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" s="30" t="s">
         <v>117</v>
-      </c>
-      <c r="C16" s="30" t="s">
-        <v>118</v>
       </c>
       <c r="H16" s="32"/>
     </row>
@@ -16263,19 +16252,19 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>120</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -16292,7 +16281,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
new card template: faq
</commit_message>
<xml_diff>
--- a/data/copy.xlsx
+++ b/data/copy.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="187">
   <si>
     <t>key</t>
   </si>
@@ -40,7 +40,7 @@
     <t>prod_state</t>
   </si>
   <si>
-    <t>after</t>
+    <t>during</t>
   </si>
   <si>
     <t>stage_state</t>
@@ -49,19 +49,16 @@
     <t>dev_state</t>
   </si>
   <si>
-    <t>during</t>
-  </si>
-  <si>
     <t>live_audio</t>
   </si>
   <si>
-    <t>live</t>
+    <t>inactive</t>
   </si>
   <si>
     <t>results_gop_footnote</t>
   </si>
   <si>
-    <t>Republicans in American Samoa also hold caucuses today.</t>
+    <t>Republicans in American Samoa also held caucuses today.</t>
   </si>
   <si>
     <t>results_dem_footnote</t>
@@ -70,7 +67,7 @@
     <t>delegates_dem_footnote</t>
   </si>
   <si>
-    <t>Democratic delegate totals include delegates determined via state primaries and caucuses and&amp;nbsp;&lt;a href="http://www.npr.org/2016/02/18/467230964/survey-clinton-maintains-massive-superdelegate-lead"&gt;superdelegates&lt;/a&gt;.</t>
+    <t>Democratic delegate totals include delegates determined via state primaries and caucuses and&amp;nbsp;&lt;a href="http://www.npr.org/2016/02/18/467230964/survey-clinton-maintains-massive-superdelegate-lead"&gt;superdelegates&lt;/a&gt;.&lt;br/&gt;&lt;br/&gt;After winners are called, state parties do not always immediately award all delegates (and AP does not always immediately account for all delegates in its estimates). Sometimes the delay is to allow for full tabulation of votes, or because there are further steps involved in the state party nomination process. See the &lt;a href="http://www.npr.org/2016/03/02/468641509/elections-2016-democratic-and-republican-delegate-tracker"&gt;NPR Delegate Tracker&lt;/a&gt; for detailed state delegate allocations, including delegates outstanding.</t>
   </si>
   <si>
     <t>delegates_gop_footnote</t>
@@ -89,6 +86,18 @@
   </si>
   <si>
     <t>&lt;p&gt;If you think so, we’d love your help. Public Radio is funded a few ways, but mostly from your donations to local public radio stations.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>wa_dem_note</t>
+  </si>
+  <si>
+    <t>Vote totals are an estimated number of delegates that will be sent to further rounds of caucuses that will formally select delegates to the national convention. In Washington, the state Democratic party did not report actual vote counts.</t>
+  </si>
+  <si>
+    <t>ak_dem_note</t>
+  </si>
+  <si>
+    <t>Vote totals are an estimated number of delegates that will be sent to the state convention to formally select delegates to the national convention. Vote counts are available from the &lt;a href="http://static1.squarespace.com/static/54bee0c9e4b0441ce96c4681/t/56f7547e27d4bdeb601fa43f/1459049599932/Alaska+2016+Democratic+Presidential+Caucus+Results+%281%29.pdf"&gt;Alaska Democratic party website&lt;/a&gt;.</t>
   </si>
   <si>
     <t>meta_description</t>
@@ -265,9 +274,6 @@
     <t>get_caught_up</t>
   </si>
   <si>
-    <t>Live audio</t>
-  </si>
-  <si>
     <t>error_headline</t>
   </si>
   <si>
@@ -388,22 +394,22 @@
     <t>states</t>
   </si>
   <si>
-    <t>Tuesday, March 22</t>
-  </si>
-  <si>
-    <t>Arizona, Idaho (D), Utah, American Samoa (R)</t>
-  </si>
-  <si>
-    <t>Saturday, March 26</t>
-  </si>
-  <si>
-    <t>Alaska (D), Hawaii (D), Washington (D)</t>
-  </si>
-  <si>
     <t>Tuesday, April 5</t>
   </si>
   <si>
     <t>Wisconsin</t>
+  </si>
+  <si>
+    <t>Saturday, April 9</t>
+  </si>
+  <si>
+    <t>Wyoming (D)</t>
+  </si>
+  <si>
+    <t>Tuesday, April 19</t>
+  </si>
+  <si>
+    <t>New York</t>
   </si>
   <si>
     <t>Puerto Rico Republican&amp;nbsp;Primary</t>
@@ -920,68 +926,78 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="4" t="s">
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="2"/>
+      <c r="A14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations>
@@ -1009,34 +1025,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="19" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="20" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="20" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="20" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5">
@@ -4986,14 +5002,6 @@
     <row r="991">
       <c r="A991" s="21"/>
       <c r="B991" s="21"/>
-    </row>
-    <row r="992">
-      <c r="A992" s="21"/>
-      <c r="B992" s="21"/>
-    </row>
-    <row r="993">
-      <c r="A993" s="21"/>
-      <c r="B993" s="21"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -5045,58 +5053,58 @@
     </row>
     <row r="2">
       <c r="A2" s="22" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="22" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="22" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="22" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="22" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -5113,77 +5121,77 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="22" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="22" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D3" s="24"/>
     </row>
     <row r="4">
       <c r="A4" s="22" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D4" s="24"/>
     </row>
     <row r="5">
       <c r="A5" s="22" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D5" s="24"/>
     </row>
     <row r="6">
       <c r="A6" s="22" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D6" s="24"/>
     </row>
@@ -5201,34 +5209,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F1" s="26"/>
       <c r="G1" s="27" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H1" s="28" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I1" s="27" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="J1" s="27" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B2" s="29" t="str">
         <f t="shared" ref="B2:B5" si="1">H2</f>
@@ -5239,11 +5247,11 @@
         <v>71.2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F2" s="31"/>
       <c r="G2" s="32" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H2" s="33">
         <v>24787.0</v>
@@ -5257,7 +5265,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B3" s="29" t="str">
         <f t="shared" si="1"/>
@@ -5269,7 +5277,7 @@
       </c>
       <c r="F3" s="31"/>
       <c r="G3" s="32" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="H3" s="33">
         <v>4479.0</v>
@@ -5283,7 +5291,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B4" s="29" t="str">
         <f t="shared" si="1"/>
@@ -5295,7 +5303,7 @@
       </c>
       <c r="F4" s="31"/>
       <c r="G4" s="32" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H4" s="33">
         <v>2903.0</v>
@@ -5309,7 +5317,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B5" s="29" t="str">
         <f t="shared" si="1"/>
@@ -5321,7 +5329,7 @@
       </c>
       <c r="F5" s="31"/>
       <c r="G5" s="32" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H5" s="33">
         <v>450.0</v>
@@ -5335,7 +5343,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B6" s="35" t="str">
         <f>sum(H6:H14)</f>
@@ -5347,7 +5355,7 @@
       </c>
       <c r="F6" s="31"/>
       <c r="G6" s="32" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="H6" s="33">
         <v>273.0</v>
@@ -5370,7 +5378,7 @@
       </c>
       <c r="F7" s="31"/>
       <c r="G7" s="32" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="H7" s="33">
         <v>229.0</v>
@@ -5386,7 +5394,7 @@
       <c r="B8" s="37"/>
       <c r="F8" s="31"/>
       <c r="G8" s="32" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="H8" s="33">
         <v>125.0</v>
@@ -5402,7 +5410,7 @@
       <c r="B9" s="37"/>
       <c r="F9" s="31"/>
       <c r="G9" s="32" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H9" s="33">
         <v>58.0</v>
@@ -5418,7 +5426,7 @@
       <c r="B10" s="37"/>
       <c r="F10" s="31"/>
       <c r="G10" s="32" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="H10" s="33">
         <v>39.0</v>
@@ -5432,21 +5440,21 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C11" s="39" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E11" s="40"/>
       <c r="F11" s="31"/>
       <c r="G11" s="32" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="H11" s="33">
         <v>28.0</v>
@@ -5460,18 +5468,18 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B12" s="39" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C12" s="39" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E12" s="40"/>
       <c r="F12" s="31"/>
       <c r="G12" s="32" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H12" s="33">
         <v>25.0</v>
@@ -5485,18 +5493,18 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C13" s="39" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E13" s="40"/>
       <c r="F13" s="31"/>
       <c r="G13" s="32" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="H13" s="33">
         <v>19.0</v>
@@ -5510,18 +5518,18 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B14" s="39" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C14" s="39" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E14" s="40"/>
       <c r="F14" s="31"/>
       <c r="G14" s="32" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="H14" s="33">
         <v>1413.0</v>
@@ -5530,28 +5538,28 @@
         <v>4.0E-4</v>
       </c>
       <c r="J14" s="32" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E15" s="40"/>
       <c r="H15" s="42"/>
     </row>
     <row r="16">
       <c r="B16" s="43" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C16" s="40" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H16" s="42"/>
     </row>
@@ -9548,10 +9556,10 @@
     </row>
     <row r="2" ht="30.0" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -9574,10 +9582,10 @@
     </row>
     <row r="3" ht="30.0" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -9600,10 +9608,10 @@
     </row>
     <row r="4" ht="30.0" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -9626,10 +9634,10 @@
     </row>
     <row r="5" ht="30.0" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -9652,10 +9660,10 @@
     </row>
     <row r="6" ht="30.0" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -9678,7 +9686,7 @@
     </row>
     <row r="7" ht="30.0" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>3</v>
@@ -9704,10 +9712,10 @@
     </row>
     <row r="8" ht="30.0" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -9730,10 +9738,10 @@
     </row>
     <row r="9" ht="30.0" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -9756,10 +9764,10 @@
     </row>
     <row r="10" ht="30.0" customHeight="1">
       <c r="A10" s="7" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -9782,10 +9790,10 @@
     </row>
     <row r="11" ht="30.0" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -9808,7 +9816,7 @@
     </row>
     <row r="12" ht="30.0" customHeight="1">
       <c r="A12" s="7" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -9832,7 +9840,7 @@
     </row>
     <row r="13" ht="30.0" customHeight="1">
       <c r="A13" s="7" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -9856,7 +9864,7 @@
     </row>
     <row r="14" ht="30.0" customHeight="1">
       <c r="A14" s="7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -9880,7 +9888,7 @@
     </row>
     <row r="15" ht="30.0" customHeight="1">
       <c r="A15" s="7" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -9904,7 +9912,7 @@
     </row>
     <row r="16" ht="30.0" customHeight="1">
       <c r="A16" s="7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -9928,7 +9936,7 @@
     </row>
     <row r="17" ht="30.0" customHeight="1">
       <c r="A17" s="7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -9952,10 +9960,10 @@
     </row>
     <row r="18" ht="30.0" customHeight="1">
       <c r="A18" s="7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
@@ -9978,10 +9986,10 @@
     </row>
     <row r="19" ht="30.0" customHeight="1">
       <c r="A19" s="7" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -10004,10 +10012,10 @@
     </row>
     <row r="20" ht="30.0" customHeight="1">
       <c r="A20" s="7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -10030,10 +10038,10 @@
     </row>
     <row r="21" ht="30.0" customHeight="1">
       <c r="A21" s="7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -11904,13 +11912,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="14" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>
@@ -11938,106 +11946,106 @@
     </row>
     <row r="2">
       <c r="A2" s="14" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -12058,117 +12066,86 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="14" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="14" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -12188,108 +12165,106 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="14" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="14" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2"/>
+        <v>67</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>65</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="C4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>67</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -12342,42 +12317,42 @@
     </row>
     <row r="2" ht="33.0" customHeight="1">
       <c r="A2" s="17" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" ht="33.0" customHeight="1">
       <c r="A3" s="17" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" ht="33.0" customHeight="1">
       <c r="A4" s="17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" ht="33.0" customHeight="1">
       <c r="A5" s="17" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" ht="33.0" customHeight="1">
       <c r="A6" s="17" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" ht="33.0" customHeight="1">
@@ -16378,58 +16353,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -16452,7 +16427,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -16481,27 +16456,27 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -16530,50 +16505,50 @@
     </row>
     <row r="2">
       <c r="A2" s="20" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="20" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="20" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="20" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="20" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="20" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8">

</xml_diff>